<commit_message>
Modif du Product BackLog avec vélocité + graphique
</commit_message>
<xml_diff>
--- a/Product_Backlog_Camping.xlsx
+++ b/Product_Backlog_Camping.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="107">
   <si>
     <t>Objectif de Produit : Un Site web de réservation d'emplacement de Camping</t>
   </si>
@@ -106,9 +106,6 @@
   </si>
   <si>
     <t>En tant qu'internaute (ou client)  je veux consulter  les emplacements par type</t>
-  </si>
-  <si>
-    <t>?</t>
   </si>
   <si>
     <t>Recherche</t>
@@ -324,9 +321,6 @@
     <t>2</t>
   </si>
   <si>
-    <t>3-4-5-6-8-9-12</t>
-  </si>
-  <si>
     <t>Fin Sprint 0</t>
   </si>
   <si>
@@ -384,7 +378,10 @@
     <t xml:space="preserve">Test </t>
   </si>
   <si>
-    <t>10</t>
+    <t>2 + X</t>
+  </si>
+  <si>
+    <t>3-4-5-6-8-9</t>
   </si>
 </sst>
 </file>
@@ -783,15 +780,6 @@
   </cellStyleXfs>
   <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -981,6 +969,15 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1656,1080 +1653,1077 @@
   </sheetPr>
   <dimension ref="A1:AMJ73"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" style="4" customWidth="1"/>
-    <col min="2" max="2" width="23.85546875" style="5" customWidth="1"/>
-    <col min="3" max="3" width="22.28515625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="31.5703125" style="6" customWidth="1"/>
-    <col min="5" max="5" width="66.85546875" style="6" customWidth="1"/>
-    <col min="6" max="6" width="31" style="7" customWidth="1"/>
-    <col min="7" max="7" width="21.42578125" style="8" customWidth="1"/>
-    <col min="8" max="8" width="13.140625" style="9" customWidth="1"/>
-    <col min="9" max="9" width="36.5703125" style="9" customWidth="1"/>
-    <col min="10" max="1024" width="9.140625" style="9"/>
+    <col min="1" max="1" width="17.42578125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="23.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="22.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="31.5703125" style="3" customWidth="1"/>
+    <col min="5" max="5" width="66.85546875" style="3" customWidth="1"/>
+    <col min="6" max="6" width="31" style="4" customWidth="1"/>
+    <col min="7" max="7" width="21.42578125" style="5" customWidth="1"/>
+    <col min="8" max="8" width="13.140625" style="6" customWidth="1"/>
+    <col min="9" max="9" width="36.5703125" style="6" customWidth="1"/>
+    <col min="10" max="1024" width="9.140625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:65" ht="81" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="3" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="72" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="4"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="1"/>
     </row>
     <row r="2" spans="1:65" ht="36" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="2" t="s">
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="73" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="G2" s="7"/>
-    </row>
-    <row r="3" spans="1:65" s="15" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="11" t="s">
+      <c r="E2" s="73"/>
+      <c r="G2" s="4"/>
+    </row>
+    <row r="3" spans="1:65" s="12" customFormat="1" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="12" t="s">
+      <c r="E3" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="13" t="s">
+      <c r="G3" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="14"/>
-      <c r="I3" s="1"/>
-      <c r="J3" s="1"/>
-      <c r="K3" s="1"/>
-      <c r="L3" s="1"/>
-      <c r="M3" s="14"/>
-      <c r="N3" s="14"/>
-      <c r="O3" s="14"/>
-      <c r="P3" s="14"/>
-      <c r="Q3" s="14"/>
-      <c r="R3" s="14"/>
-      <c r="S3" s="14"/>
-      <c r="T3" s="14"/>
-      <c r="U3" s="14"/>
-      <c r="V3" s="14"/>
-      <c r="W3" s="14"/>
-      <c r="X3" s="14"/>
-      <c r="Y3" s="14"/>
-      <c r="Z3" s="14"/>
-      <c r="AA3" s="14"/>
-      <c r="AB3" s="14"/>
-      <c r="AC3" s="14"/>
-      <c r="AD3" s="14"/>
-      <c r="AE3" s="14"/>
-      <c r="AF3" s="14"/>
-      <c r="AG3" s="14"/>
-      <c r="AH3" s="14"/>
-      <c r="AI3" s="14"/>
-      <c r="AJ3" s="14"/>
-      <c r="AK3" s="14"/>
-      <c r="AL3" s="14"/>
-      <c r="AM3" s="14"/>
-      <c r="AN3" s="14"/>
-      <c r="AO3" s="14"/>
-      <c r="AP3" s="14"/>
-      <c r="AQ3" s="14"/>
-      <c r="AR3" s="14"/>
-      <c r="AS3" s="14"/>
-      <c r="AT3" s="14"/>
-      <c r="AU3" s="14"/>
-      <c r="AV3" s="14"/>
-      <c r="AW3" s="14"/>
-      <c r="AX3" s="14"/>
-      <c r="AY3" s="14"/>
-      <c r="AZ3" s="14"/>
-      <c r="BA3" s="14"/>
-      <c r="BB3" s="14"/>
-      <c r="BC3" s="14"/>
-      <c r="BD3" s="14"/>
-      <c r="BE3" s="14"/>
-      <c r="BF3" s="14"/>
-      <c r="BG3" s="14"/>
-      <c r="BH3" s="14"/>
-      <c r="BI3" s="14"/>
-      <c r="BJ3" s="14"/>
-      <c r="BK3" s="14"/>
-      <c r="BL3" s="14"/>
-      <c r="BM3" s="14"/>
-    </row>
-    <row r="4" spans="1:65" s="20" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="16">
+      <c r="H3" s="11"/>
+      <c r="I3" s="74"/>
+      <c r="J3" s="74"/>
+      <c r="K3" s="74"/>
+      <c r="L3" s="74"/>
+      <c r="M3" s="11"/>
+      <c r="N3" s="11"/>
+      <c r="O3" s="11"/>
+      <c r="P3" s="11"/>
+      <c r="Q3" s="11"/>
+      <c r="R3" s="11"/>
+      <c r="S3" s="11"/>
+      <c r="T3" s="11"/>
+      <c r="U3" s="11"/>
+      <c r="V3" s="11"/>
+      <c r="W3" s="11"/>
+      <c r="X3" s="11"/>
+      <c r="Y3" s="11"/>
+      <c r="Z3" s="11"/>
+      <c r="AA3" s="11"/>
+      <c r="AB3" s="11"/>
+      <c r="AC3" s="11"/>
+      <c r="AD3" s="11"/>
+      <c r="AE3" s="11"/>
+      <c r="AF3" s="11"/>
+      <c r="AG3" s="11"/>
+      <c r="AH3" s="11"/>
+      <c r="AI3" s="11"/>
+      <c r="AJ3" s="11"/>
+      <c r="AK3" s="11"/>
+      <c r="AL3" s="11"/>
+      <c r="AM3" s="11"/>
+      <c r="AN3" s="11"/>
+      <c r="AO3" s="11"/>
+      <c r="AP3" s="11"/>
+      <c r="AQ3" s="11"/>
+      <c r="AR3" s="11"/>
+      <c r="AS3" s="11"/>
+      <c r="AT3" s="11"/>
+      <c r="AU3" s="11"/>
+      <c r="AV3" s="11"/>
+      <c r="AW3" s="11"/>
+      <c r="AX3" s="11"/>
+      <c r="AY3" s="11"/>
+      <c r="AZ3" s="11"/>
+      <c r="BA3" s="11"/>
+      <c r="BB3" s="11"/>
+      <c r="BC3" s="11"/>
+      <c r="BD3" s="11"/>
+      <c r="BE3" s="11"/>
+      <c r="BF3" s="11"/>
+      <c r="BG3" s="11"/>
+      <c r="BH3" s="11"/>
+      <c r="BI3" s="11"/>
+      <c r="BJ3" s="11"/>
+      <c r="BK3" s="11"/>
+      <c r="BL3" s="11"/>
+      <c r="BM3" s="11"/>
+    </row>
+    <row r="4" spans="1:65" s="17" customFormat="1" ht="80.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="13">
         <v>1</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="14">
         <v>350</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="C4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="F4" s="18"/>
-      <c r="G4" s="19">
+      <c r="F4" s="15"/>
+      <c r="G4" s="16">
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:65" s="20" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="21">
+    <row r="5" spans="1:65" s="17" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="18">
         <f t="shared" ref="A5:A28" si="0">A4+1</f>
         <v>2</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="19">
         <v>340</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="21" t="s">
+      <c r="D5" s="18" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="21" t="s">
+      <c r="E5" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="24">
+      <c r="F5" s="20"/>
+      <c r="G5" s="21">
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:65" s="20" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="21">
+    <row r="6" spans="1:65" s="17" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="18">
         <f t="shared" si="0"/>
         <v>3</v>
       </c>
-      <c r="B6" s="22">
+      <c r="B6" s="19">
         <v>300</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D6" s="21" t="s">
+      <c r="D6" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="21" t="s">
+      <c r="E6" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="24">
+      <c r="F6" s="20"/>
+      <c r="G6" s="21">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:65" s="20" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="21">
+    <row r="7" spans="1:65" s="17" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="18">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B7" s="22">
+      <c r="B7" s="19">
         <v>250</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="19" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="21" t="s">
+      <c r="D7" s="18" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="21" t="s">
+      <c r="E7" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="24">
+      <c r="F7" s="20"/>
+      <c r="G7" s="21">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:65" s="26" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="21">
+    <row r="8" spans="1:65" s="23" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="18">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B8" s="22">
+      <c r="B8" s="19">
         <v>220</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="21" t="s">
+      <c r="D8" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="21" t="s">
+      <c r="E8" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="F8" s="25"/>
-      <c r="G8" s="24">
+      <c r="F8" s="22"/>
+      <c r="G8" s="21">
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:65" s="26" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="21">
+    <row r="9" spans="1:65" s="23" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="18">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="14">
         <v>200</v>
       </c>
-      <c r="C9" s="22" t="s">
+      <c r="C9" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="D9" s="21" t="s">
+      <c r="D9" s="18" t="s">
         <v>23</v>
       </c>
-      <c r="E9" s="21" t="s">
+      <c r="E9" s="18" t="s">
         <v>24</v>
       </c>
-      <c r="F9" s="25"/>
-      <c r="G9" s="19">
+      <c r="F9" s="22"/>
+      <c r="G9" s="16">
         <v>2</v>
       </c>
-      <c r="H9" s="26" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:65" s="26" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="21">
+    </row>
+    <row r="10" spans="1:65" s="23" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="18">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B10" s="22">
+      <c r="B10" s="19">
         <v>180</v>
       </c>
-      <c r="C10" s="22" t="s">
+      <c r="C10" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="E10" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="E10" s="21" t="s">
-        <v>28</v>
-      </c>
-      <c r="F10" s="23"/>
-      <c r="G10" s="24">
+      <c r="F10" s="20"/>
+      <c r="G10" s="21">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:65" s="26" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="21">
+    <row r="11" spans="1:65" s="23" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="18">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="19">
         <v>150</v>
       </c>
-      <c r="C11" s="22" t="s">
+      <c r="C11" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="21" t="s">
+      <c r="D11" s="18" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="E11" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="F11" s="23"/>
-      <c r="G11" s="24">
+      <c r="F11" s="20"/>
+      <c r="G11" s="21">
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:65" s="26" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="21">
+    <row r="12" spans="1:65" s="23" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="18">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B12" s="22">
+      <c r="B12" s="19">
         <v>140</v>
       </c>
-      <c r="C12" s="22" t="s">
+      <c r="C12" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="E12" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="E12" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="F12" s="23"/>
-      <c r="G12" s="24">
+      <c r="F12" s="20"/>
+      <c r="G12" s="21">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:65" s="26" customFormat="1" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="21">
+    <row r="13" spans="1:65" s="23" customFormat="1" ht="110.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="18">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B13" s="22">
+      <c r="B13" s="19">
         <v>120</v>
       </c>
-      <c r="C13" s="22" t="s">
+      <c r="C13" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D13" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="E13" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="E13" s="21" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="16"/>
-      <c r="G13" s="24">
+      <c r="F13" s="13"/>
+      <c r="G13" s="21">
         <v>13</v>
       </c>
     </row>
-    <row r="14" spans="1:65" s="26" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="21">
+    <row r="14" spans="1:65" s="23" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="18">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B14" s="17">
+      <c r="B14" s="14">
         <v>110</v>
       </c>
-      <c r="C14" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D14" s="21" t="s">
+      <c r="C14" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="E14" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="21" t="s">
-        <v>37</v>
-      </c>
-      <c r="F14" s="25"/>
-      <c r="G14" s="19">
+      <c r="F14" s="22"/>
+      <c r="G14" s="16">
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="1:65" s="26" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="21">
+    <row r="15" spans="1:65" s="23" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="18">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B15" s="17">
+      <c r="B15" s="14">
         <v>90</v>
       </c>
-      <c r="C15" s="22" t="s">
+      <c r="C15" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D15" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="E15" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="21" t="s">
-        <v>40</v>
-      </c>
-      <c r="F15" s="25"/>
-      <c r="G15" s="19">
+      <c r="F15" s="22"/>
+      <c r="G15" s="16">
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:65" s="26" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="21">
+    <row r="16" spans="1:65" s="23" customFormat="1" ht="69" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="18">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B16" s="17">
+      <c r="B16" s="14">
         <v>85</v>
       </c>
-      <c r="C16" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D16" s="21" t="s">
+      <c r="C16" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D16" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="E16" s="21" t="s">
-        <v>42</v>
-      </c>
-      <c r="F16" s="25"/>
-      <c r="G16" s="19">
+      <c r="F16" s="22"/>
+      <c r="G16" s="16">
         <v>5</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="26" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="21">
+    <row r="17" spans="1:7" s="23" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="18">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B17" s="17">
+      <c r="B17" s="14">
         <v>80</v>
       </c>
-      <c r="C17" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D17" s="16" t="s">
+      <c r="C17" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>42</v>
+      </c>
+      <c r="E17" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="E17" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="F17" s="25"/>
-      <c r="G17" s="24">
+      <c r="F17" s="22"/>
+      <c r="G17" s="21">
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:7" s="26" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="21">
+    <row r="18" spans="1:7" s="23" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A18" s="18">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B18" s="17">
+      <c r="B18" s="14">
         <v>70</v>
       </c>
-      <c r="C18" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="D18" s="16" t="s">
+      <c r="C18" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="18" t="s">
         <v>45</v>
       </c>
-      <c r="E18" s="21" t="s">
-        <v>46</v>
-      </c>
-      <c r="F18" s="25"/>
-      <c r="G18" s="24">
+      <c r="F18" s="22"/>
+      <c r="G18" s="21">
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="26" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="21">
+    <row r="19" spans="1:7" s="23" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="18">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B19" s="17">
+      <c r="B19" s="14">
         <v>65</v>
       </c>
-      <c r="C19" s="22" t="s">
+      <c r="C19" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D19" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="D19" s="16" t="s">
+      <c r="E19" s="18" t="s">
         <v>48</v>
       </c>
-      <c r="E19" s="21" t="s">
-        <v>49</v>
-      </c>
-      <c r="F19" s="25"/>
-      <c r="G19" s="24">
+      <c r="F19" s="22"/>
+      <c r="G19" s="21">
         <v>3</v>
       </c>
     </row>
-    <row r="20" spans="1:7" s="26" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="21">
+    <row r="20" spans="1:7" s="23" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="18">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B20" s="17">
+      <c r="B20" s="14">
         <v>60</v>
       </c>
-      <c r="C20" s="22" t="s">
-        <v>47</v>
-      </c>
-      <c r="D20" s="16" t="s">
+      <c r="C20" s="19" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>49</v>
+      </c>
+      <c r="E20" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="E20" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="F20" s="25"/>
-      <c r="G20" s="24">
+      <c r="F20" s="22"/>
+      <c r="G20" s="21">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:7" s="26" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="21">
+    <row r="21" spans="1:7" s="23" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="18">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B21" s="22">
+      <c r="B21" s="19">
         <v>50</v>
       </c>
-      <c r="C21" s="22" t="s">
+      <c r="C21" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D21" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="D21" s="21" t="s">
+      <c r="E21" s="18" t="s">
         <v>53</v>
       </c>
-      <c r="E21" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="F21" s="23"/>
-      <c r="G21" s="24">
+      <c r="F21" s="20"/>
+      <c r="G21" s="21">
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:7" s="26" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="21">
+    <row r="22" spans="1:7" s="23" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="18">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B22" s="22">
+      <c r="B22" s="19">
         <v>40</v>
       </c>
-      <c r="C22" s="22" t="s">
+      <c r="C22" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="D22" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="D22" s="21" t="s">
+      <c r="E22" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="E22" s="21" t="s">
-        <v>57</v>
-      </c>
-      <c r="F22" s="23"/>
-      <c r="G22" s="24">
+      <c r="F22" s="20"/>
+      <c r="G22" s="21">
         <v>5</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="26" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="21">
+    <row r="23" spans="1:7" s="23" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="18">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B23" s="17">
+      <c r="B23" s="14">
         <v>30</v>
       </c>
-      <c r="C23" s="22" t="s">
+      <c r="C23" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="D23" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="D23" s="21" t="s">
+      <c r="E23" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="E23" s="21" t="s">
-        <v>60</v>
-      </c>
-      <c r="F23" s="25"/>
-      <c r="G23" s="24">
+      <c r="F23" s="22"/>
+      <c r="G23" s="21">
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="26" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="21">
+    <row r="24" spans="1:7" s="23" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="18">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B24" s="22">
+      <c r="B24" s="19">
         <v>28</v>
       </c>
-      <c r="C24" s="22" t="s">
+      <c r="C24" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="D24" s="18" t="s">
         <v>61</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="E24" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="E24" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="F24" s="23"/>
-      <c r="G24" s="24">
+      <c r="F24" s="20"/>
+      <c r="G24" s="21">
         <v>5</v>
       </c>
     </row>
-    <row r="25" spans="1:7" s="26" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="21">
+    <row r="25" spans="1:7" s="23" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="18">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B25" s="22">
+      <c r="B25" s="19">
         <v>25</v>
       </c>
-      <c r="C25" s="22" t="s">
+      <c r="C25" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="18" t="s">
         <v>64</v>
       </c>
-      <c r="D25" s="21" t="s">
+      <c r="E25" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="E25" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="F25" s="23"/>
-      <c r="G25" s="24">
+      <c r="F25" s="20"/>
+      <c r="G25" s="21">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="26" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="21">
+    <row r="26" spans="1:7" s="23" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="18">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B26" s="22">
+      <c r="B26" s="19">
         <v>22</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="19" t="s">
+        <v>66</v>
+      </c>
+      <c r="D26" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="D26" s="21" t="s">
+      <c r="E26" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="E26" s="21" t="s">
-        <v>69</v>
-      </c>
-      <c r="F26" s="23"/>
-      <c r="G26" s="24">
+      <c r="F26" s="20"/>
+      <c r="G26" s="21">
         <v>5</v>
       </c>
     </row>
-    <row r="27" spans="1:7" s="28" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="21">
+    <row r="27" spans="1:7" s="25" customFormat="1" ht="60.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="18">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B27" s="22">
+      <c r="B27" s="19">
         <v>20</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D27" s="18" t="s">
         <v>70</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="E27" s="24" t="s">
         <v>71</v>
       </c>
-      <c r="E27" s="27" t="s">
-        <v>72</v>
-      </c>
-      <c r="F27" s="23"/>
-      <c r="G27" s="24">
+      <c r="F27" s="20"/>
+      <c r="G27" s="21">
         <v>13</v>
       </c>
     </row>
-    <row r="28" spans="1:7" s="28" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="21">
+    <row r="28" spans="1:7" s="25" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="18">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B28" s="17">
+      <c r="B28" s="14">
         <v>18</v>
       </c>
-      <c r="C28" s="17" t="s">
-        <v>33</v>
-      </c>
-      <c r="D28" s="16" t="s">
+      <c r="C28" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="D28" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="E28" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="E28" s="16" t="s">
-        <v>74</v>
-      </c>
-      <c r="F28" s="25"/>
-      <c r="G28" s="19">
+      <c r="F28" s="22"/>
+      <c r="G28" s="16">
         <v>3</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="28" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="21"/>
-      <c r="B29" s="22"/>
-      <c r="C29" s="22"/>
-      <c r="D29" s="21"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="23"/>
-      <c r="G29" s="29"/>
-    </row>
-    <row r="30" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="30"/>
-      <c r="B30" s="31"/>
-      <c r="C30" s="31"/>
-      <c r="D30" s="32"/>
-      <c r="E30" s="32"/>
-      <c r="F30" s="33"/>
-      <c r="G30" s="34"/>
-    </row>
-    <row r="31" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="10"/>
-      <c r="B31" s="10"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="35"/>
-      <c r="E31" s="35"/>
-      <c r="F31" s="36"/>
-      <c r="G31" s="10"/>
-    </row>
-    <row r="32" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="30"/>
-      <c r="B32" s="31"/>
-      <c r="C32" s="31"/>
-      <c r="D32" s="32"/>
-      <c r="E32" s="32"/>
-      <c r="F32" s="33"/>
-      <c r="G32" s="34"/>
-    </row>
-    <row r="33" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="30"/>
-      <c r="B33" s="31"/>
-      <c r="C33" s="31"/>
-      <c r="D33" s="32"/>
-      <c r="E33" s="32"/>
-      <c r="F33" s="33"/>
-      <c r="G33" s="34"/>
-    </row>
-    <row r="34" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="10"/>
-      <c r="B34" s="10"/>
-      <c r="C34" s="10"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="36"/>
-      <c r="G34" s="10"/>
-    </row>
-    <row r="35" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="30"/>
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32"/>
-      <c r="F35" s="33"/>
-      <c r="G35" s="34"/>
-    </row>
-    <row r="36" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="30"/>
-      <c r="B36" s="31"/>
-      <c r="C36" s="31"/>
-      <c r="D36" s="32"/>
-      <c r="E36" s="32"/>
-      <c r="F36" s="33"/>
-      <c r="G36" s="34"/>
-    </row>
-    <row r="37" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="10"/>
-      <c r="B37" s="10"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="35"/>
-      <c r="E37" s="35"/>
-      <c r="F37" s="36"/>
-      <c r="G37" s="10"/>
-    </row>
-    <row r="38" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="30"/>
-      <c r="B38" s="31"/>
-      <c r="C38" s="31"/>
-      <c r="D38" s="32"/>
-      <c r="E38" s="32"/>
-      <c r="F38" s="33"/>
-      <c r="G38" s="34"/>
-    </row>
-    <row r="39" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="30"/>
-      <c r="B39" s="31"/>
-      <c r="C39" s="31"/>
-      <c r="D39" s="32"/>
-      <c r="E39" s="32"/>
-      <c r="F39" s="33"/>
-      <c r="G39" s="34"/>
-    </row>
-    <row r="40" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="10"/>
-      <c r="B40" s="10"/>
-      <c r="C40" s="10"/>
-      <c r="D40" s="35"/>
-      <c r="E40" s="35"/>
-      <c r="F40" s="36"/>
-      <c r="G40" s="10"/>
-    </row>
-    <row r="41" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="30"/>
-      <c r="B41" s="31"/>
-      <c r="C41" s="31"/>
-      <c r="D41" s="32"/>
-      <c r="E41" s="32"/>
-      <c r="F41" s="33"/>
-      <c r="G41" s="34"/>
-    </row>
-    <row r="42" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="30"/>
-      <c r="B42" s="31"/>
-      <c r="C42" s="31"/>
-      <c r="D42" s="32"/>
-      <c r="E42" s="32"/>
-      <c r="F42" s="33"/>
-      <c r="G42" s="34"/>
-    </row>
-    <row r="43" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="10"/>
-      <c r="B43" s="10"/>
-      <c r="C43" s="10"/>
-      <c r="D43" s="35"/>
-      <c r="E43" s="35"/>
-      <c r="F43" s="36"/>
-      <c r="G43" s="10"/>
-    </row>
-    <row r="44" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="30"/>
-      <c r="B44" s="31"/>
-      <c r="C44" s="31"/>
-      <c r="D44" s="32"/>
-      <c r="E44" s="32"/>
-      <c r="F44" s="33"/>
-      <c r="G44" s="34"/>
-    </row>
-    <row r="45" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="30"/>
-      <c r="B45" s="31"/>
-      <c r="C45" s="31"/>
-      <c r="D45" s="32"/>
-      <c r="E45" s="32"/>
-      <c r="F45" s="33"/>
-      <c r="G45" s="34"/>
-    </row>
-    <row r="46" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="10"/>
-      <c r="B46" s="10"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="35"/>
-      <c r="E46" s="35"/>
-      <c r="F46" s="36"/>
-      <c r="G46" s="10"/>
-    </row>
-    <row r="47" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="30"/>
-      <c r="B47" s="31"/>
-      <c r="C47" s="31"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="32"/>
-      <c r="F47" s="33"/>
-      <c r="G47" s="34"/>
-    </row>
-    <row r="48" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="30"/>
-      <c r="B48" s="31"/>
-      <c r="C48" s="31"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="32"/>
-      <c r="F48" s="33"/>
-      <c r="G48" s="34"/>
-    </row>
-    <row r="49" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="10"/>
-      <c r="B49" s="10"/>
-      <c r="C49" s="10"/>
-      <c r="D49" s="35"/>
-      <c r="E49" s="35"/>
-      <c r="F49" s="36"/>
-      <c r="G49" s="10"/>
-    </row>
-    <row r="50" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="30"/>
-      <c r="B50" s="31"/>
-      <c r="C50" s="31"/>
-      <c r="D50" s="32"/>
-      <c r="E50" s="32"/>
-      <c r="F50" s="33"/>
-      <c r="G50" s="34"/>
-    </row>
-    <row r="51" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="30"/>
-      <c r="B51" s="31"/>
-      <c r="C51" s="31"/>
-      <c r="D51" s="32"/>
-      <c r="E51" s="32"/>
-      <c r="F51" s="33"/>
-      <c r="G51" s="34"/>
-    </row>
-    <row r="52" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="10"/>
-      <c r="B52" s="10"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="35"/>
-      <c r="E52" s="35"/>
-      <c r="F52" s="36"/>
-      <c r="G52" s="10"/>
-    </row>
-    <row r="53" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="30"/>
-      <c r="B53" s="31"/>
-      <c r="C53" s="31"/>
-      <c r="D53" s="32"/>
-      <c r="E53" s="32"/>
-      <c r="F53" s="33"/>
-      <c r="G53" s="34"/>
-    </row>
-    <row r="54" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="30"/>
-      <c r="B54" s="31"/>
-      <c r="C54" s="31"/>
-      <c r="D54" s="32"/>
-      <c r="E54" s="32"/>
-      <c r="F54" s="33"/>
-      <c r="G54" s="34"/>
-    </row>
-    <row r="55" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="10"/>
-      <c r="B55" s="10"/>
-      <c r="C55" s="10"/>
-      <c r="D55" s="35"/>
-      <c r="E55" s="35"/>
-      <c r="F55" s="36"/>
-      <c r="G55" s="10"/>
-    </row>
-    <row r="56" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="30"/>
-      <c r="B56" s="31"/>
-      <c r="C56" s="31"/>
-      <c r="D56" s="32"/>
-      <c r="E56" s="32"/>
-      <c r="F56" s="33"/>
-      <c r="G56" s="34"/>
-    </row>
-    <row r="57" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="30"/>
-      <c r="B57" s="31"/>
-      <c r="C57" s="31"/>
-      <c r="D57" s="32"/>
-      <c r="E57" s="32"/>
-      <c r="F57" s="33"/>
-      <c r="G57" s="34"/>
-    </row>
-    <row r="58" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="10"/>
-      <c r="B58" s="10"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="35"/>
-      <c r="E58" s="35"/>
-      <c r="F58" s="36"/>
-      <c r="G58" s="10"/>
-    </row>
-    <row r="59" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="30"/>
-      <c r="B59" s="31"/>
-      <c r="C59" s="31"/>
-      <c r="D59" s="32"/>
-      <c r="E59" s="32"/>
-      <c r="F59" s="33"/>
-      <c r="G59" s="34"/>
-    </row>
-    <row r="60" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="30"/>
-      <c r="B60" s="31"/>
-      <c r="C60" s="31"/>
-      <c r="D60" s="32"/>
-      <c r="E60" s="32"/>
-      <c r="F60" s="33"/>
-      <c r="G60" s="34"/>
-    </row>
-    <row r="61" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="10"/>
-      <c r="B61" s="10"/>
-      <c r="C61" s="10"/>
-      <c r="D61" s="35"/>
-      <c r="E61" s="35"/>
-      <c r="F61" s="36"/>
-      <c r="G61" s="10"/>
-    </row>
-    <row r="62" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="30"/>
-      <c r="B62" s="31"/>
-      <c r="C62" s="31"/>
-      <c r="D62" s="32"/>
-      <c r="E62" s="32"/>
-      <c r="F62" s="33"/>
-      <c r="G62" s="34"/>
-    </row>
-    <row r="63" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="30"/>
-      <c r="B63" s="31"/>
-      <c r="C63" s="31"/>
-      <c r="D63" s="32"/>
-      <c r="E63" s="32"/>
-      <c r="F63" s="33"/>
-      <c r="G63" s="34"/>
-    </row>
-    <row r="64" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="10"/>
-      <c r="B64" s="10"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="35"/>
-      <c r="E64" s="35"/>
-      <c r="F64" s="36"/>
-      <c r="G64" s="10"/>
-    </row>
-    <row r="65" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="30"/>
-      <c r="B65" s="31"/>
-      <c r="C65" s="31"/>
-      <c r="D65" s="32"/>
-      <c r="E65" s="32"/>
-      <c r="F65" s="33"/>
-      <c r="G65" s="34"/>
-    </row>
-    <row r="66" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="30"/>
-      <c r="B66" s="31"/>
-      <c r="C66" s="31"/>
-      <c r="D66" s="32"/>
-      <c r="E66" s="32"/>
-      <c r="F66" s="33"/>
-      <c r="G66" s="34"/>
-    </row>
-    <row r="67" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="10"/>
-      <c r="B67" s="10"/>
-      <c r="C67" s="10"/>
-      <c r="D67" s="35"/>
-      <c r="E67" s="35"/>
-      <c r="F67" s="36"/>
-      <c r="G67" s="10"/>
-    </row>
-    <row r="68" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="30"/>
-      <c r="B68" s="31"/>
-      <c r="C68" s="31"/>
-      <c r="D68" s="32"/>
-      <c r="E68" s="32"/>
-      <c r="F68" s="33"/>
-      <c r="G68" s="34"/>
-    </row>
-    <row r="69" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="30"/>
-      <c r="B69" s="31"/>
-      <c r="C69" s="31"/>
-      <c r="D69" s="32"/>
-      <c r="E69" s="32"/>
-      <c r="F69" s="33"/>
-      <c r="G69" s="34"/>
-    </row>
-    <row r="70" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="10"/>
-      <c r="B70" s="10"/>
-      <c r="C70" s="10"/>
-      <c r="D70" s="35"/>
-      <c r="E70" s="35"/>
-      <c r="F70" s="36"/>
-      <c r="G70" s="10"/>
-    </row>
-    <row r="71" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="37"/>
-      <c r="B71" s="10"/>
-      <c r="C71" s="10"/>
-      <c r="D71" s="35"/>
-      <c r="E71" s="35"/>
-      <c r="F71" s="36"/>
-      <c r="G71" s="38"/>
-    </row>
-    <row r="72" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="37"/>
-      <c r="B72" s="10"/>
-      <c r="C72" s="10"/>
-      <c r="D72" s="35"/>
-      <c r="E72" s="35"/>
-      <c r="F72" s="36"/>
-      <c r="G72" s="38"/>
-    </row>
-    <row r="73" spans="1:7" s="28" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A73" s="37"/>
-      <c r="B73" s="10"/>
-      <c r="C73" s="10"/>
-      <c r="D73" s="35"/>
-      <c r="E73" s="35"/>
-      <c r="F73" s="36"/>
-      <c r="G73" s="38"/>
+    <row r="29" spans="1:7" s="25" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="18"/>
+      <c r="B29" s="19"/>
+      <c r="C29" s="19"/>
+      <c r="D29" s="18"/>
+      <c r="E29" s="18"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="26"/>
+    </row>
+    <row r="30" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="27"/>
+      <c r="B30" s="28"/>
+      <c r="C30" s="28"/>
+      <c r="D30" s="29"/>
+      <c r="E30" s="29"/>
+      <c r="F30" s="30"/>
+      <c r="G30" s="31"/>
+    </row>
+    <row r="31" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="32"/>
+      <c r="E31" s="32"/>
+      <c r="F31" s="33"/>
+      <c r="G31" s="7"/>
+    </row>
+    <row r="32" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A32" s="27"/>
+      <c r="B32" s="28"/>
+      <c r="C32" s="28"/>
+      <c r="D32" s="29"/>
+      <c r="E32" s="29"/>
+      <c r="F32" s="30"/>
+      <c r="G32" s="31"/>
+    </row>
+    <row r="33" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A33" s="27"/>
+      <c r="B33" s="28"/>
+      <c r="C33" s="28"/>
+      <c r="D33" s="29"/>
+      <c r="E33" s="29"/>
+      <c r="F33" s="30"/>
+      <c r="G33" s="31"/>
+    </row>
+    <row r="34" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="7"/>
+      <c r="D34" s="32"/>
+      <c r="E34" s="32"/>
+      <c r="F34" s="33"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="27"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="28"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="30"/>
+      <c r="G35" s="31"/>
+    </row>
+    <row r="36" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A36" s="27"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="28"/>
+      <c r="D36" s="29"/>
+      <c r="E36" s="29"/>
+      <c r="F36" s="30"/>
+      <c r="G36" s="31"/>
+    </row>
+    <row r="37" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A37" s="7"/>
+      <c r="B37" s="7"/>
+      <c r="C37" s="7"/>
+      <c r="D37" s="32"/>
+      <c r="E37" s="32"/>
+      <c r="F37" s="33"/>
+      <c r="G37" s="7"/>
+    </row>
+    <row r="38" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A38" s="27"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="28"/>
+      <c r="D38" s="29"/>
+      <c r="E38" s="29"/>
+      <c r="F38" s="30"/>
+      <c r="G38" s="31"/>
+    </row>
+    <row r="39" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="27"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="28"/>
+      <c r="D39" s="29"/>
+      <c r="E39" s="29"/>
+      <c r="F39" s="30"/>
+      <c r="G39" s="31"/>
+    </row>
+    <row r="40" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A40" s="7"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="32"/>
+      <c r="E40" s="32"/>
+      <c r="F40" s="33"/>
+      <c r="G40" s="7"/>
+    </row>
+    <row r="41" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A41" s="27"/>
+      <c r="B41" s="28"/>
+      <c r="C41" s="28"/>
+      <c r="D41" s="29"/>
+      <c r="E41" s="29"/>
+      <c r="F41" s="30"/>
+      <c r="G41" s="31"/>
+    </row>
+    <row r="42" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A42" s="27"/>
+      <c r="B42" s="28"/>
+      <c r="C42" s="28"/>
+      <c r="D42" s="29"/>
+      <c r="E42" s="29"/>
+      <c r="F42" s="30"/>
+      <c r="G42" s="31"/>
+    </row>
+    <row r="43" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A43" s="7"/>
+      <c r="B43" s="7"/>
+      <c r="C43" s="7"/>
+      <c r="D43" s="32"/>
+      <c r="E43" s="32"/>
+      <c r="F43" s="33"/>
+      <c r="G43" s="7"/>
+    </row>
+    <row r="44" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A44" s="27"/>
+      <c r="B44" s="28"/>
+      <c r="C44" s="28"/>
+      <c r="D44" s="29"/>
+      <c r="E44" s="29"/>
+      <c r="F44" s="30"/>
+      <c r="G44" s="31"/>
+    </row>
+    <row r="45" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A45" s="27"/>
+      <c r="B45" s="28"/>
+      <c r="C45" s="28"/>
+      <c r="D45" s="29"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="30"/>
+      <c r="G45" s="31"/>
+    </row>
+    <row r="46" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="7"/>
+      <c r="B46" s="7"/>
+      <c r="C46" s="7"/>
+      <c r="D46" s="32"/>
+      <c r="E46" s="32"/>
+      <c r="F46" s="33"/>
+      <c r="G46" s="7"/>
+    </row>
+    <row r="47" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A47" s="27"/>
+      <c r="B47" s="28"/>
+      <c r="C47" s="28"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="30"/>
+      <c r="G47" s="31"/>
+    </row>
+    <row r="48" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A48" s="27"/>
+      <c r="B48" s="28"/>
+      <c r="C48" s="28"/>
+      <c r="D48" s="29"/>
+      <c r="E48" s="29"/>
+      <c r="F48" s="30"/>
+      <c r="G48" s="31"/>
+    </row>
+    <row r="49" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="7"/>
+      <c r="B49" s="7"/>
+      <c r="C49" s="7"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="32"/>
+      <c r="F49" s="33"/>
+      <c r="G49" s="7"/>
+    </row>
+    <row r="50" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A50" s="27"/>
+      <c r="B50" s="28"/>
+      <c r="C50" s="28"/>
+      <c r="D50" s="29"/>
+      <c r="E50" s="29"/>
+      <c r="F50" s="30"/>
+      <c r="G50" s="31"/>
+    </row>
+    <row r="51" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A51" s="27"/>
+      <c r="B51" s="28"/>
+      <c r="C51" s="28"/>
+      <c r="D51" s="29"/>
+      <c r="E51" s="29"/>
+      <c r="F51" s="30"/>
+      <c r="G51" s="31"/>
+    </row>
+    <row r="52" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="7"/>
+      <c r="B52" s="7"/>
+      <c r="C52" s="7"/>
+      <c r="D52" s="32"/>
+      <c r="E52" s="32"/>
+      <c r="F52" s="33"/>
+      <c r="G52" s="7"/>
+    </row>
+    <row r="53" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="27"/>
+      <c r="B53" s="28"/>
+      <c r="C53" s="28"/>
+      <c r="D53" s="29"/>
+      <c r="E53" s="29"/>
+      <c r="F53" s="30"/>
+      <c r="G53" s="31"/>
+    </row>
+    <row r="54" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="27"/>
+      <c r="B54" s="28"/>
+      <c r="C54" s="28"/>
+      <c r="D54" s="29"/>
+      <c r="E54" s="29"/>
+      <c r="F54" s="30"/>
+      <c r="G54" s="31"/>
+    </row>
+    <row r="55" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A55" s="7"/>
+      <c r="B55" s="7"/>
+      <c r="C55" s="7"/>
+      <c r="D55" s="32"/>
+      <c r="E55" s="32"/>
+      <c r="F55" s="33"/>
+      <c r="G55" s="7"/>
+    </row>
+    <row r="56" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A56" s="27"/>
+      <c r="B56" s="28"/>
+      <c r="C56" s="28"/>
+      <c r="D56" s="29"/>
+      <c r="E56" s="29"/>
+      <c r="F56" s="30"/>
+      <c r="G56" s="31"/>
+    </row>
+    <row r="57" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="27"/>
+      <c r="B57" s="28"/>
+      <c r="C57" s="28"/>
+      <c r="D57" s="29"/>
+      <c r="E57" s="29"/>
+      <c r="F57" s="30"/>
+      <c r="G57" s="31"/>
+    </row>
+    <row r="58" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A58" s="7"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="32"/>
+      <c r="E58" s="32"/>
+      <c r="F58" s="33"/>
+      <c r="G58" s="7"/>
+    </row>
+    <row r="59" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A59" s="27"/>
+      <c r="B59" s="28"/>
+      <c r="C59" s="28"/>
+      <c r="D59" s="29"/>
+      <c r="E59" s="29"/>
+      <c r="F59" s="30"/>
+      <c r="G59" s="31"/>
+    </row>
+    <row r="60" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="27"/>
+      <c r="B60" s="28"/>
+      <c r="C60" s="28"/>
+      <c r="D60" s="29"/>
+      <c r="E60" s="29"/>
+      <c r="F60" s="30"/>
+      <c r="G60" s="31"/>
+    </row>
+    <row r="61" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="7"/>
+      <c r="B61" s="7"/>
+      <c r="C61" s="7"/>
+      <c r="D61" s="32"/>
+      <c r="E61" s="32"/>
+      <c r="F61" s="33"/>
+      <c r="G61" s="7"/>
+    </row>
+    <row r="62" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="27"/>
+      <c r="B62" s="28"/>
+      <c r="C62" s="28"/>
+      <c r="D62" s="29"/>
+      <c r="E62" s="29"/>
+      <c r="F62" s="30"/>
+      <c r="G62" s="31"/>
+    </row>
+    <row r="63" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="27"/>
+      <c r="B63" s="28"/>
+      <c r="C63" s="28"/>
+      <c r="D63" s="29"/>
+      <c r="E63" s="29"/>
+      <c r="F63" s="30"/>
+      <c r="G63" s="31"/>
+    </row>
+    <row r="64" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A64" s="7"/>
+      <c r="B64" s="7"/>
+      <c r="C64" s="7"/>
+      <c r="D64" s="32"/>
+      <c r="E64" s="32"/>
+      <c r="F64" s="33"/>
+      <c r="G64" s="7"/>
+    </row>
+    <row r="65" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A65" s="27"/>
+      <c r="B65" s="28"/>
+      <c r="C65" s="28"/>
+      <c r="D65" s="29"/>
+      <c r="E65" s="29"/>
+      <c r="F65" s="30"/>
+      <c r="G65" s="31"/>
+    </row>
+    <row r="66" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A66" s="27"/>
+      <c r="B66" s="28"/>
+      <c r="C66" s="28"/>
+      <c r="D66" s="29"/>
+      <c r="E66" s="29"/>
+      <c r="F66" s="30"/>
+      <c r="G66" s="31"/>
+    </row>
+    <row r="67" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A67" s="7"/>
+      <c r="B67" s="7"/>
+      <c r="C67" s="7"/>
+      <c r="D67" s="32"/>
+      <c r="E67" s="32"/>
+      <c r="F67" s="33"/>
+      <c r="G67" s="7"/>
+    </row>
+    <row r="68" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A68" s="27"/>
+      <c r="B68" s="28"/>
+      <c r="C68" s="28"/>
+      <c r="D68" s="29"/>
+      <c r="E68" s="29"/>
+      <c r="F68" s="30"/>
+      <c r="G68" s="31"/>
+    </row>
+    <row r="69" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A69" s="27"/>
+      <c r="B69" s="28"/>
+      <c r="C69" s="28"/>
+      <c r="D69" s="29"/>
+      <c r="E69" s="29"/>
+      <c r="F69" s="30"/>
+      <c r="G69" s="31"/>
+    </row>
+    <row r="70" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A70" s="7"/>
+      <c r="B70" s="7"/>
+      <c r="C70" s="7"/>
+      <c r="D70" s="32"/>
+      <c r="E70" s="32"/>
+      <c r="F70" s="33"/>
+      <c r="G70" s="7"/>
+    </row>
+    <row r="71" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A71" s="34"/>
+      <c r="B71" s="7"/>
+      <c r="C71" s="7"/>
+      <c r="D71" s="32"/>
+      <c r="E71" s="32"/>
+      <c r="F71" s="33"/>
+      <c r="G71" s="35"/>
+    </row>
+    <row r="72" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A72" s="34"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="7"/>
+      <c r="D72" s="32"/>
+      <c r="E72" s="32"/>
+      <c r="F72" s="33"/>
+      <c r="G72" s="35"/>
+    </row>
+    <row r="73" spans="1:7" s="25" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="34"/>
+      <c r="B73" s="7"/>
+      <c r="C73" s="7"/>
+      <c r="D73" s="32"/>
+      <c r="E73" s="32"/>
+      <c r="F73" s="33"/>
+      <c r="G73" s="35"/>
     </row>
   </sheetData>
   <autoFilter ref="A3:G53"/>
@@ -2751,164 +2745,166 @@
   <dimension ref="A1:AMJ12"/>
   <sheetViews>
     <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="30.140625" style="39" customWidth="1"/>
-    <col min="3" max="4" width="30.7109375" style="40" customWidth="1"/>
-    <col min="5" max="5" width="11.42578125" style="41"/>
-    <col min="6" max="6" width="34.28515625" style="41" customWidth="1"/>
-    <col min="7" max="7" width="44.42578125" style="41" customWidth="1"/>
-    <col min="8" max="1024" width="11.42578125" style="41"/>
+    <col min="1" max="2" width="30.140625" style="36" customWidth="1"/>
+    <col min="3" max="4" width="30.7109375" style="37" customWidth="1"/>
+    <col min="5" max="5" width="11.42578125" style="38"/>
+    <col min="6" max="6" width="34.28515625" style="38" customWidth="1"/>
+    <col min="7" max="7" width="44.42578125" style="38" customWidth="1"/>
+    <col min="8" max="1024" width="11.42578125" style="38"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="39" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="40"/>
+      <c r="B3" s="41" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3" s="43"/>
-      <c r="B3" s="44" t="s">
+      <c r="C3" s="42" t="s">
         <v>76</v>
       </c>
-      <c r="C3" s="45" t="s">
+      <c r="D3" s="42" t="s">
         <v>77</v>
       </c>
-      <c r="D3" s="45" t="s">
+      <c r="F3" s="39" t="s">
         <v>78</v>
       </c>
-      <c r="F3" s="42" t="s">
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="40"/>
+      <c r="B4" s="43" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="43"/>
-      <c r="B4" s="46" t="s">
+      <c r="C4" s="44"/>
+      <c r="D4" s="45"/>
+      <c r="F4" s="37"/>
+      <c r="G4" s="37"/>
+    </row>
+    <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A5" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="48"/>
-      <c r="F4" s="40"/>
-      <c r="G4" s="40"/>
-    </row>
-    <row r="5" spans="1:7" ht="90" x14ac:dyDescent="0.25">
-      <c r="A5" s="49" t="s">
+      <c r="B5" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="50" t="s">
+      <c r="C5" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="51" t="s">
+      <c r="D5" s="49"/>
+      <c r="F5" s="50" t="s">
         <v>83</v>
       </c>
-      <c r="D5" s="52"/>
-      <c r="F5" s="53" t="s">
+      <c r="G5" s="50">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="46" t="s">
         <v>84</v>
       </c>
-      <c r="G5" s="53">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="49" t="s">
+      <c r="B6" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="B6" s="50" t="s">
+      <c r="C6" s="48" t="s">
+        <v>106</v>
+      </c>
+      <c r="D6" s="49"/>
+      <c r="F6" s="50" t="s">
         <v>86</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="G6" s="50">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="D6" s="52"/>
-      <c r="F6" s="53" t="s">
+      <c r="B7" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="C7" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="G6" s="53">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="49" t="s">
+      <c r="D7" s="49"/>
+      <c r="F7" s="50" t="s">
         <v>89</v>
       </c>
-      <c r="B7" s="50" t="s">
-        <v>107</v>
-      </c>
-      <c r="C7" s="51" t="s">
+      <c r="G7" s="50"/>
+    </row>
+    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="52"/>
-      <c r="F7" s="53" t="s">
+      <c r="B8" s="47"/>
+      <c r="C8" s="48"/>
+      <c r="D8" s="49"/>
+      <c r="F8" s="50" t="s">
         <v>91</v>
       </c>
-      <c r="G7" s="53"/>
-    </row>
-    <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="49" t="s">
+      <c r="G8" s="50">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="B8" s="50"/>
-      <c r="C8" s="51"/>
-      <c r="D8" s="52"/>
-      <c r="F8" s="53" t="s">
+      <c r="B9" s="47"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="52"/>
+      <c r="F9" s="50" t="s">
         <v>93</v>
       </c>
-      <c r="G8" s="53">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="30.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="49" t="s">
+      <c r="G9" s="50">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A10" s="46" t="s">
         <v>94</v>
       </c>
-      <c r="B9" s="50"/>
-      <c r="C9" s="54"/>
-      <c r="D9" s="55"/>
-      <c r="F9" s="53" t="s">
+      <c r="B10" s="47" t="s">
         <v>95</v>
       </c>
-      <c r="G9" s="53">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A10" s="49" t="s">
+      <c r="C10" s="51"/>
+      <c r="D10" s="52"/>
+      <c r="F10" s="50" t="s">
         <v>96</v>
       </c>
-      <c r="B10" s="50" t="s">
+      <c r="G10" s="50"/>
+    </row>
+    <row r="11" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="C10" s="54"/>
-      <c r="D10" s="55"/>
-      <c r="F10" s="53" t="s">
+      <c r="B11" s="47" t="s">
+        <v>85</v>
+      </c>
+      <c r="C11" s="51"/>
+      <c r="D11" s="52"/>
+      <c r="F11" s="53"/>
+      <c r="G11" s="53"/>
+    </row>
+    <row r="12" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="A12" s="46" t="s">
         <v>98</v>
       </c>
-      <c r="G10" s="53"/>
-    </row>
-    <row r="11" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="49" t="s">
-        <v>99</v>
-      </c>
-      <c r="B11" s="50" t="s">
-        <v>86</v>
-      </c>
-      <c r="C11" s="54"/>
-      <c r="D11" s="55"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="56"/>
-    </row>
-    <row r="12" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="A12" s="49" t="s">
-        <v>100</v>
-      </c>
-      <c r="B12" s="57" t="s">
-        <v>86</v>
-      </c>
-      <c r="C12" s="58"/>
-      <c r="D12" s="59"/>
+      <c r="B12" s="54" t="s">
+        <v>85</v>
+      </c>
+      <c r="C12" s="55" t="s">
+        <v>105</v>
+      </c>
+      <c r="D12" s="56"/>
     </row>
   </sheetData>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="0.98402777777777795" bottom="0.98402777777777795" header="0.51180555555555496" footer="0.51180555555555496"/>
@@ -2935,161 +2931,161 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="60" t="s">
+      <c r="A1" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="B1" s="58"/>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="59"/>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="60"/>
+      <c r="B2" s="61"/>
+      <c r="C2" s="61"/>
+      <c r="D2" s="62" t="s">
+        <v>100</v>
+      </c>
+      <c r="E2" s="63"/>
+    </row>
+    <row r="3" spans="1:5" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="60"/>
+      <c r="B3" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="B1" s="61"/>
-      <c r="C1" s="61"/>
-      <c r="D1" s="61"/>
-      <c r="E1" s="62"/>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="63"/>
-      <c r="B2" s="64"/>
-      <c r="C2" s="64"/>
-      <c r="D2" s="65" t="s">
+      <c r="C3" s="61"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="63"/>
+    </row>
+    <row r="4" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="60"/>
+      <c r="B4" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="66"/>
-    </row>
-    <row r="3" spans="1:5" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="63"/>
-      <c r="B3" s="67" t="s">
+      <c r="C4" s="61"/>
+      <c r="D4" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="C3" s="64"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="66"/>
-    </row>
-    <row r="4" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="63"/>
-      <c r="B4" s="64" t="s">
+      <c r="E4" s="63"/>
+    </row>
+    <row r="5" spans="1:5" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="60"/>
+      <c r="B5" s="66"/>
+      <c r="C5" s="61"/>
+      <c r="D5" s="67"/>
+      <c r="E5" s="63"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="60"/>
+      <c r="B6" s="61"/>
+      <c r="C6" s="61"/>
+      <c r="D6" s="61"/>
+      <c r="E6" s="63"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="60"/>
+      <c r="B7" s="62" t="s">
         <v>104</v>
       </c>
-      <c r="C4" s="64"/>
-      <c r="D4" s="65" t="s">
-        <v>105</v>
-      </c>
-      <c r="E4" s="66"/>
-    </row>
-    <row r="5" spans="1:5" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="63"/>
-      <c r="B5" s="69"/>
-      <c r="C5" s="64"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="66"/>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="63"/>
-      <c r="B6" s="64"/>
-      <c r="C6" s="64"/>
-      <c r="D6" s="64"/>
-      <c r="E6" s="66"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="63"/>
-      <c r="B7" s="65" t="s">
-        <v>106</v>
-      </c>
-      <c r="C7" s="64"/>
-      <c r="D7" s="64"/>
-      <c r="E7" s="66"/>
+      <c r="C7" s="61"/>
+      <c r="D7" s="61"/>
+      <c r="E7" s="63"/>
     </row>
     <row r="8" spans="1:5" ht="75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="63"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="64"/>
-      <c r="D8" s="64"/>
-      <c r="E8" s="66"/>
+      <c r="A8" s="60"/>
+      <c r="B8" s="68"/>
+      <c r="C8" s="61"/>
+      <c r="D8" s="61"/>
+      <c r="E8" s="63"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="72"/>
-      <c r="B9" s="73"/>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="74"/>
+      <c r="A9" s="69"/>
+      <c r="B9" s="70"/>
+      <c r="C9" s="70"/>
+      <c r="D9" s="70"/>
+      <c r="E9" s="71"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="63"/>
-      <c r="B10" s="64"/>
-      <c r="C10" s="64"/>
-      <c r="D10" s="64"/>
-      <c r="E10" s="66"/>
+      <c r="A10" s="60"/>
+      <c r="B10" s="61"/>
+      <c r="C10" s="61"/>
+      <c r="D10" s="61"/>
+      <c r="E10" s="63"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="57" t="s">
+        <v>99</v>
+      </c>
+      <c r="B11" s="58"/>
+      <c r="C11" s="58"/>
+      <c r="D11" s="58"/>
+      <c r="E11" s="59"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="60"/>
+      <c r="B12" s="61"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="62" t="s">
+        <v>100</v>
+      </c>
+      <c r="E12" s="63"/>
+    </row>
+    <row r="13" spans="1:5" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="60"/>
+      <c r="B13" s="64" t="s">
         <v>101</v>
       </c>
-      <c r="B11" s="61"/>
-      <c r="C11" s="61"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="62"/>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A12" s="63"/>
-      <c r="B12" s="64"/>
-      <c r="C12" s="64"/>
-      <c r="D12" s="65" t="s">
+      <c r="C13" s="61"/>
+      <c r="D13" s="65"/>
+      <c r="E13" s="63"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="60"/>
+      <c r="B14" s="61" t="s">
         <v>102</v>
       </c>
-      <c r="E12" s="66"/>
-    </row>
-    <row r="13" spans="1:5" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="63"/>
-      <c r="B13" s="67" t="s">
+      <c r="C14" s="61"/>
+      <c r="D14" s="62" t="s">
         <v>103</v>
       </c>
-      <c r="C13" s="64"/>
-      <c r="D13" s="68"/>
-      <c r="E13" s="66"/>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A14" s="63"/>
-      <c r="B14" s="64" t="s">
+      <c r="E14" s="63"/>
+    </row>
+    <row r="15" spans="1:5" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="60"/>
+      <c r="B15" s="66"/>
+      <c r="C15" s="61"/>
+      <c r="D15" s="67"/>
+      <c r="E15" s="63"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="60"/>
+      <c r="B16" s="61"/>
+      <c r="C16" s="61"/>
+      <c r="D16" s="61"/>
+      <c r="E16" s="63"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="60"/>
+      <c r="B17" s="62" t="s">
         <v>104</v>
       </c>
-      <c r="C14" s="64"/>
-      <c r="D14" s="65" t="s">
-        <v>105</v>
-      </c>
-      <c r="E14" s="66"/>
-    </row>
-    <row r="15" spans="1:5" ht="67.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="63"/>
-      <c r="B15" s="69"/>
-      <c r="C15" s="64"/>
-      <c r="D15" s="70"/>
-      <c r="E15" s="66"/>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A16" s="63"/>
-      <c r="B16" s="64"/>
-      <c r="C16" s="64"/>
-      <c r="D16" s="64"/>
-      <c r="E16" s="66"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A17" s="63"/>
-      <c r="B17" s="65" t="s">
-        <v>106</v>
-      </c>
-      <c r="C17" s="64"/>
-      <c r="D17" s="64"/>
-      <c r="E17" s="66"/>
+      <c r="C17" s="61"/>
+      <c r="D17" s="61"/>
+      <c r="E17" s="63"/>
     </row>
     <row r="18" spans="1:5" ht="70.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="63"/>
-      <c r="B18" s="71"/>
-      <c r="C18" s="64"/>
-      <c r="D18" s="64"/>
-      <c r="E18" s="66"/>
+      <c r="A18" s="60"/>
+      <c r="B18" s="68"/>
+      <c r="C18" s="61"/>
+      <c r="D18" s="61"/>
+      <c r="E18" s="63"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A19" s="72"/>
-      <c r="B19" s="73"/>
-      <c r="C19" s="73"/>
-      <c r="D19" s="73"/>
-      <c r="E19" s="74"/>
+      <c r="A19" s="69"/>
+      <c r="B19" s="70"/>
+      <c r="C19" s="70"/>
+      <c r="D19" s="70"/>
+      <c r="E19" s="71"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51180555555555496" footer="0.51180555555555496"/>

</xml_diff>

<commit_message>
Mise a jour product backlog Sprint 1
</commit_message>
<xml_diff>
--- a/Product_Backlog_Camping.xlsx
+++ b/Product_Backlog_Camping.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="109">
   <si>
     <t>Objectif de Produit : Un Site web de réservation d'emplacement de Camping</t>
   </si>
@@ -327,9 +327,6 @@
     <t>Vélocité prévue</t>
   </si>
   <si>
-    <t>20</t>
-  </si>
-  <si>
     <t>Fin Sprint 1</t>
   </si>
   <si>
@@ -378,10 +375,19 @@
     <t xml:space="preserve">Test </t>
   </si>
   <si>
-    <t>2 + X</t>
-  </si>
-  <si>
     <t>3-4-5-6-8-9</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>3-4-Admin</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>15</t>
   </si>
 </sst>
 </file>
@@ -1653,8 +1659,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2744,8 +2750,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ12"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -2814,7 +2820,7 @@
         <v>85</v>
       </c>
       <c r="C6" s="48" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D6" s="49"/>
       <c r="F6" s="50" t="s">
@@ -2832,23 +2838,23 @@
         <v>85</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>88</v>
+        <v>105</v>
       </c>
       <c r="D7" s="49"/>
       <c r="F7" s="50" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G7" s="50"/>
     </row>
     <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B8" s="47"/>
       <c r="C8" s="48"/>
       <c r="D8" s="49"/>
       <c r="F8" s="50" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="G8" s="50">
         <v>35</v>
@@ -2856,13 +2862,13 @@
     </row>
     <row r="9" spans="1:7" ht="30.75" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="46" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B9" s="47"/>
       <c r="C9" s="51"/>
       <c r="D9" s="52"/>
       <c r="F9" s="50" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="G9" s="50">
         <v>20</v>
@@ -2870,39 +2876,43 @@
     </row>
     <row r="10" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A10" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="B10" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="B10" s="47" t="s">
-        <v>95</v>
-      </c>
-      <c r="C10" s="51"/>
+      <c r="C10" s="51" t="s">
+        <v>106</v>
+      </c>
       <c r="D10" s="52"/>
       <c r="F10" s="50" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G10" s="50"/>
     </row>
     <row r="11" spans="1:7" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="46" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B11" s="47" t="s">
         <v>85</v>
       </c>
-      <c r="C11" s="51"/>
+      <c r="C11" s="51" t="s">
+        <v>107</v>
+      </c>
       <c r="D11" s="52"/>
       <c r="F11" s="53"/>
       <c r="G11" s="53"/>
     </row>
     <row r="12" spans="1:7" ht="20.25" x14ac:dyDescent="0.25">
       <c r="A12" s="46" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B12" s="54" t="s">
         <v>85</v>
       </c>
       <c r="C12" s="55" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D12" s="56"/>
     </row>
@@ -2932,7 +2942,7 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="57" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B1" s="58"/>
       <c r="C1" s="58"/>
@@ -2944,14 +2954,14 @@
       <c r="B2" s="61"/>
       <c r="C2" s="61"/>
       <c r="D2" s="62" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E2" s="63"/>
     </row>
     <row r="3" spans="1:5" ht="71.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="60"/>
       <c r="B3" s="64" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C3" s="61"/>
       <c r="D3" s="65"/>
@@ -2960,11 +2970,11 @@
     <row r="4" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="60"/>
       <c r="B4" s="61" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C4" s="61"/>
       <c r="D4" s="62" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E4" s="63"/>
     </row>
@@ -2985,7 +2995,7 @@
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="60"/>
       <c r="B7" s="62" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C7" s="61"/>
       <c r="D7" s="61"/>
@@ -3014,7 +3024,7 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="57" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B11" s="58"/>
       <c r="C11" s="58"/>
@@ -3026,14 +3036,14 @@
       <c r="B12" s="61"/>
       <c r="C12" s="61"/>
       <c r="D12" s="62" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E12" s="63"/>
     </row>
     <row r="13" spans="1:5" ht="82.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="60"/>
       <c r="B13" s="64" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C13" s="61"/>
       <c r="D13" s="65"/>
@@ -3042,11 +3052,11 @@
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="60"/>
       <c r="B14" s="61" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C14" s="61"/>
       <c r="D14" s="62" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E14" s="63"/>
     </row>
@@ -3067,7 +3077,7 @@
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="60"/>
       <c r="B17" s="62" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C17" s="61"/>
       <c r="D17" s="61"/>

</xml_diff>

<commit_message>
Mise a jour product backlog Sprint1 encore
</commit_message>
<xml_diff>
--- a/Product_Backlog_Camping.xlsx
+++ b/Product_Backlog_Camping.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -384,10 +384,10 @@
     <t>3-4-Admin</t>
   </si>
   <si>
-    <t>13</t>
-  </si>
-  <si>
     <t>15</t>
+  </si>
+  <si>
+    <t>17</t>
   </si>
 </sst>
 </file>
@@ -1210,6 +1210,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>107</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>92</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1659,8 +1662,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ73"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2750,8 +2753,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -2844,7 +2847,9 @@
       <c r="F7" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="G7" s="50"/>
+      <c r="G7" s="50">
+        <v>92</v>
+      </c>
     </row>
     <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
       <c r="A8" s="46" t="s">

</xml_diff>

<commit_message>
Mise a jour vélocité prévu product backlog
</commit_message>
<xml_diff>
--- a/Product_Backlog_Camping.xlsx
+++ b/Product_Backlog_Camping.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -378,9 +378,6 @@
     <t>3-4-5-6-8-9</t>
   </si>
   <si>
-    <t>12</t>
-  </si>
-  <si>
     <t>3-4-Admin</t>
   </si>
   <si>
@@ -388,6 +385,9 @@
   </si>
   <si>
     <t>17</t>
+  </si>
+  <si>
+    <t>18</t>
   </si>
 </sst>
 </file>
@@ -1662,7 +1662,7 @@
   </sheetPr>
   <dimension ref="A1:AMJ73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -2753,8 +2753,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ12"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -2841,7 +2841,7 @@
         <v>85</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="D7" s="49"/>
       <c r="F7" s="50" t="s">
@@ -2887,7 +2887,7 @@
         <v>94</v>
       </c>
       <c r="C10" s="51" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D10" s="52"/>
       <c r="F10" s="50" t="s">
@@ -2903,7 +2903,7 @@
         <v>85</v>
       </c>
       <c r="C11" s="51" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D11" s="52"/>
       <c r="F11" s="53"/>
@@ -2917,7 +2917,7 @@
         <v>85</v>
       </c>
       <c r="C12" s="55" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D12" s="56"/>
     </row>

</xml_diff>

<commit_message>
mise a jour product backlog apres revue du prof
</commit_message>
<xml_diff>
--- a/Product_Backlog_Camping.xlsx
+++ b/Product_Backlog_Camping.xlsx
@@ -378,16 +378,16 @@
     <t>3-4-5-6-8-9</t>
   </si>
   <si>
-    <t>3-4-Admin</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>17</t>
-  </si>
-  <si>
     <t>16</t>
+  </si>
+  <si>
+    <t>3-4</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>8</t>
   </si>
 </sst>
 </file>
@@ -1212,7 +1212,7 @@
                   <c:v>107</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>92</c:v>
+                  <c:v>101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1662,8 +1662,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ73"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2754,7 +2754,7 @@
   <dimension ref="A1:AMJ12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -2820,7 +2820,7 @@
         <v>84</v>
       </c>
       <c r="B6" s="47" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="C6" s="48" t="s">
         <v>104</v>
@@ -2841,14 +2841,14 @@
         <v>85</v>
       </c>
       <c r="C7" s="48" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="D7" s="49"/>
       <c r="F7" s="50" t="s">
         <v>88</v>
       </c>
       <c r="G7" s="50">
-        <v>92</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
@@ -2887,7 +2887,7 @@
         <v>94</v>
       </c>
       <c r="C10" s="51" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="D10" s="52"/>
       <c r="F10" s="50" t="s">
@@ -2903,7 +2903,7 @@
         <v>85</v>
       </c>
       <c r="C11" s="51" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="D11" s="52"/>
       <c r="F11" s="53"/>
@@ -2917,7 +2917,7 @@
         <v>85</v>
       </c>
       <c r="C12" s="55" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="D12" s="56"/>
     </row>

</xml_diff>

<commit_message>
fix du product backlog vous pouvez look pour vos user story
</commit_message>
<xml_diff>
--- a/Product_Backlog_Camping.xlsx
+++ b/Product_Backlog_Camping.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="112">
   <si>
     <t>Objectif de Produit : Un Site web de réservation d'emplacement de Camping</t>
   </si>
@@ -390,7 +390,13 @@
     <t>8</t>
   </si>
   <si>
-    <t>5-6-7-8-9</t>
+    <t>5-6-7-8-9-10-11-12-13-14-15-16-17-18-19-20-21-22-23</t>
+  </si>
+  <si>
+    <t>70</t>
+  </si>
+  <si>
+    <t>5-6-7-8-9-</t>
   </si>
 </sst>
 </file>
@@ -1665,8 +1671,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1869,6 +1875,10 @@
       <c r="G7" s="21">
         <v>2</v>
       </c>
+      <c r="I7" s="17">
+        <f>SUM(G8:G26)-G15</f>
+        <v>82</v>
+      </c>
     </row>
     <row r="8" spans="1:65" s="23" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="18">
@@ -2180,7 +2190,7 @@
     </row>
     <row r="22" spans="1:7" s="23" customFormat="1" ht="62.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="18">
-        <f t="shared" si="0"/>
+        <f>A21+1</f>
         <v>19</v>
       </c>
       <c r="B22" s="19">
@@ -2202,7 +2212,7 @@
     </row>
     <row r="23" spans="1:7" s="23" customFormat="1" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="18">
-        <f t="shared" si="0"/>
+        <f>A22+1</f>
         <v>20</v>
       </c>
       <c r="B23" s="14">
@@ -2756,8 +2766,8 @@
   </sheetPr>
   <dimension ref="A1:AMJ12"/>
   <sheetViews>
-    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -2818,7 +2828,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="54" x14ac:dyDescent="0.25">
       <c r="A6" s="46" t="s">
         <v>84</v>
       </c>
@@ -2848,7 +2858,9 @@
       <c r="C7" s="48" t="s">
         <v>105</v>
       </c>
-      <c r="D7" s="49"/>
+      <c r="D7" s="49" t="s">
+        <v>110</v>
+      </c>
       <c r="F7" s="50" t="s">
         <v>88</v>
       </c>
@@ -2894,7 +2906,9 @@
       <c r="C10" s="51" t="s">
         <v>106</v>
       </c>
-      <c r="D10" s="52"/>
+      <c r="D10" s="52" t="s">
+        <v>111</v>
+      </c>
       <c r="F10" s="50" t="s">
         <v>95</v>
       </c>

</xml_diff>